<commit_message>
Adding PySPark Data Source Properties File
</commit_message>
<xml_diff>
--- a/Databricks_Notes.xlsx
+++ b/Databricks_Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Confidential\data-cloudops-natvie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA45D46C-6987-4929-A9D3-2CAF01DE7F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D3D00C-BC7C-41A4-B25E-06218ECAB371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{6D06DD71-AA96-4A60-BF7F-1C9189E66ACB}"/>
   </bookViews>
@@ -3060,215 +3060,214 @@
     </r>
   </si>
   <si>
+    <t>Enable AQE to dynamically coalesce partitions post-shuffle.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>spark.sql.adaptive.coalescePartitions.enabled = true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Use Delta Lake Cloning for Zero-Copy Copies</t>
+  </si>
+  <si>
+    <t>Create zero-copy clones for testing or development.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>CREATE TABLE table_clone CLONE table_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Define: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>CREATE LIVE TABLE my_table AS SELECT ...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>g4dn.xlarge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for ML training.</t>
+    </r>
+  </si>
+  <si>
+    <t>Leverage Unity Catalog for Metadata Optimization</t>
+  </si>
+  <si>
+    <t>Centralize metadata management to reduce overhead.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Migrate tables to Unity Catalog: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>CREATE CATALOG my_catalog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Optimize Workflow Scheduling with Job Clusters</t>
+  </si>
+  <si>
+    <t>Use job-specific clusters for workflows to minimize waste.</t>
+  </si>
+  <si>
+    <t>Configure Workflow to use a new job cluster per run.</t>
+  </si>
+  <si>
+    <t>Use Databricks Advisor for Automated Recommendations</t>
+  </si>
+  <si>
+    <t>Get automated performance and cost optimization suggestions.</t>
+  </si>
+  <si>
+    <t>Review Advisor recommendations in Databricks SQL UI.</t>
+  </si>
+  <si>
+    <t>☁️Cluster Configuration &amp; Scaling</t>
+  </si>
+  <si>
+    <t>💾Data Storage &amp; Layout Optimization</t>
+  </si>
+  <si>
+    <t>⚡Query Execution &amp; Optimization</t>
+  </si>
+  <si>
+    <t>🔥Spark-Specific Tuning</t>
+  </si>
+  <si>
+    <t>🌊Delta Lake Features</t>
+  </si>
+  <si>
+    <t>🚀Advanced Optimization Techniques</t>
+  </si>
+  <si>
+    <t>💰Cost &amp; Resource Management</t>
+  </si>
+  <si>
+    <t>⏳Streaming &amp; Real-Time Workloads</t>
+  </si>
+  <si>
+    <t>🔗External Data &amp; Integrations</t>
+  </si>
+  <si>
+    <t>🐍Language &amp; Environment</t>
+  </si>
+  <si>
+    <t>🔒Security &amp; Governance</t>
+  </si>
+  <si>
+    <t>🔍Monitoring &amp; Debugging</t>
+  </si>
+  <si>
+    <t>🤖Machine Learning</t>
+  </si>
+  <si>
+    <t>🛠️Miscellaneous</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Tune </t>
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial Unicode MS"/>
       </rPr>
       <t>spark.sql.adaptive.coalescePartitions.enabled</t>
     </r>
-  </si>
-  <si>
-    <t>Enable AQE to dynamically coalesce partitions post-shuffle.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>spark.sql.adaptive.coalescePartitions.enabled = true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>Use Delta Lake Cloning for Zero-Copy Copies</t>
-  </si>
-  <si>
-    <t>Create zero-copy clones for testing or development.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Run: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>CREATE TABLE table_clone CLONE table_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Define: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>CREATE LIVE TABLE my_table AS SELECT ...</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Select </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>g4dn.xlarge</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for ML training.</t>
-    </r>
-  </si>
-  <si>
-    <t>Leverage Unity Catalog for Metadata Optimization</t>
-  </si>
-  <si>
-    <t>Centralize metadata management to reduce overhead.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Migrate tables to Unity Catalog: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>CREATE CATALOG my_catalog</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>Optimize Workflow Scheduling with Job Clusters</t>
-  </si>
-  <si>
-    <t>Use job-specific clusters for workflows to minimize waste.</t>
-  </si>
-  <si>
-    <t>Configure Workflow to use a new job cluster per run.</t>
-  </si>
-  <si>
-    <t>Use Databricks Advisor for Automated Recommendations</t>
-  </si>
-  <si>
-    <t>Get automated performance and cost optimization suggestions.</t>
-  </si>
-  <si>
-    <t>Review Advisor recommendations in Databricks SQL UI.</t>
-  </si>
-  <si>
-    <t>☁️Cluster Configuration &amp; Scaling</t>
-  </si>
-  <si>
-    <t>💾Data Storage &amp; Layout Optimization</t>
-  </si>
-  <si>
-    <t>⚡Query Execution &amp; Optimization</t>
-  </si>
-  <si>
-    <t>🔥Spark-Specific Tuning</t>
-  </si>
-  <si>
-    <t>🌊Delta Lake Features</t>
-  </si>
-  <si>
-    <t>🚀Advanced Optimization Techniques</t>
-  </si>
-  <si>
-    <t>💰Cost &amp; Resource Management</t>
-  </si>
-  <si>
-    <t>⏳Streaming &amp; Real-Time Workloads</t>
-  </si>
-  <si>
-    <t>🔗External Data &amp; Integrations</t>
-  </si>
-  <si>
-    <t>🐍Language &amp; Environment</t>
-  </si>
-  <si>
-    <t>🔒Security &amp; Governance</t>
-  </si>
-  <si>
-    <t>🔍Monitoring &amp; Debugging</t>
-  </si>
-  <si>
-    <t>🤖Machine Learning</t>
-  </si>
-  <si>
-    <t>🛠️Miscellaneous</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3296,12 +3295,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3471,23 +3464,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3495,14 +3478,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3525,8 +3502,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3845,1516 +3846,1516 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.5">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="13"/>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="13"/>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="13"/>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="13"/>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="13"/>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="13"/>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="13"/>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="13"/>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="13"/>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="13"/>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.5">
+      <c r="A14" s="13"/>
+      <c r="B14" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="9"/>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="9"/>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="9"/>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="9"/>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="9"/>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="9"/>
-      <c r="B10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="9"/>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="9"/>
-      <c r="B12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="9"/>
-      <c r="B13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.5">
-      <c r="A14" s="9"/>
-      <c r="B14" s="19" t="s">
-        <v>332</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>333</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="9" t="s">
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="13"/>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="13"/>
+      <c r="B17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="13"/>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="13"/>
+      <c r="B19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="13"/>
+      <c r="B20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="13"/>
+      <c r="B21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="13"/>
+      <c r="B22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="13"/>
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="13"/>
+      <c r="B24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="13"/>
+      <c r="B25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="13"/>
+      <c r="B26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="13"/>
+      <c r="B27" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="13"/>
+      <c r="B28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="13"/>
+      <c r="B29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="13"/>
+      <c r="B30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="13"/>
+      <c r="B31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="13"/>
+      <c r="B32" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="9"/>
-      <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="9"/>
-      <c r="B17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="9"/>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="9"/>
-      <c r="B19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="9"/>
-      <c r="B20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="9"/>
-      <c r="B21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="9"/>
-      <c r="B22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="9"/>
-      <c r="B23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="B33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="13"/>
+      <c r="B34" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="13"/>
+      <c r="B35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="13"/>
+      <c r="B36" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="13"/>
+      <c r="B37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="13"/>
+      <c r="B38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="13"/>
+      <c r="B39" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="13"/>
+      <c r="B40" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="13"/>
+      <c r="B41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="13"/>
+      <c r="B42" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="13"/>
+      <c r="B43" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="13"/>
+      <c r="B44" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="13"/>
+      <c r="B45" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="13"/>
+      <c r="B46" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="13"/>
+      <c r="B47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="13"/>
+      <c r="B48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="13"/>
+      <c r="B49" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="13"/>
+      <c r="B51" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="13"/>
+      <c r="B52" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="13"/>
+      <c r="B53" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="13"/>
+      <c r="B54" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="13"/>
+      <c r="B55" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="13"/>
+      <c r="B56" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="13"/>
+      <c r="B57" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="13"/>
+      <c r="B58" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="13"/>
+      <c r="B59" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="13"/>
+      <c r="B60" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="13"/>
+      <c r="B62" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="13"/>
+      <c r="B63" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="13"/>
+      <c r="B64" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="13"/>
+      <c r="B65" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="13"/>
+      <c r="B66" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="13"/>
+      <c r="B67" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="13"/>
+      <c r="B68" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="13"/>
+      <c r="B69" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="13"/>
+      <c r="B70" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="13"/>
+      <c r="B72" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="13"/>
+      <c r="B73" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="13"/>
+      <c r="B74" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="13"/>
+      <c r="B75" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="13"/>
+      <c r="B76" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="13"/>
+      <c r="B77" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="9"/>
-      <c r="B29" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="9"/>
-      <c r="B30" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="9"/>
-      <c r="B31" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="9"/>
-      <c r="B32" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="9"/>
-      <c r="B34" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="9"/>
-      <c r="B35" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="9"/>
-      <c r="B36" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="9"/>
-      <c r="B37" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="9"/>
-      <c r="B38" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="9"/>
-      <c r="B39" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="9"/>
-      <c r="B40" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="9"/>
-      <c r="B41" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="9"/>
-      <c r="B42" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="9"/>
-      <c r="B43" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="9"/>
-      <c r="B44" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="9"/>
-      <c r="B45" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="9"/>
-      <c r="B46" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="9"/>
-      <c r="B47" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="9"/>
-      <c r="B48" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="9"/>
-      <c r="B49" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="9"/>
-      <c r="B51" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="9"/>
-      <c r="B52" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="9"/>
-      <c r="B53" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D53" s="10" t="s">
+    <row r="78" spans="1:4">
+      <c r="A78" s="13"/>
+      <c r="B78" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="13"/>
+      <c r="B80" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="13"/>
+      <c r="B81" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="13"/>
+      <c r="B82" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="13"/>
+      <c r="B83" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="13"/>
+      <c r="B84" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="13"/>
+      <c r="B85" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="13"/>
+      <c r="B87" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="13"/>
+      <c r="B88" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="13"/>
+      <c r="B89" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="13"/>
+      <c r="B90" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="13"/>
+      <c r="B91" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="13"/>
+      <c r="B93" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="13"/>
+      <c r="B94" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="13"/>
+      <c r="B95" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="13"/>
+      <c r="B96" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="13"/>
+      <c r="B97" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D97" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="9"/>
-      <c r="B54" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="9"/>
-      <c r="B55" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="9"/>
-      <c r="B56" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="9"/>
-      <c r="B57" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="9"/>
-      <c r="B58" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="9"/>
-      <c r="B59" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="9"/>
-      <c r="B60" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="9"/>
-      <c r="B62" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="9"/>
-      <c r="B63" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="9"/>
-      <c r="B64" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="9"/>
-      <c r="B65" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="9"/>
-      <c r="B66" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="9"/>
-      <c r="B67" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="9"/>
-      <c r="B68" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="9"/>
-      <c r="B69" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="9"/>
-      <c r="B70" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="9"/>
-      <c r="B72" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="9"/>
-      <c r="B73" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="9"/>
-      <c r="B74" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D74" s="10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="9"/>
-      <c r="B75" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D75" s="10" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="9"/>
-      <c r="B76" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D76" s="10" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="9"/>
-      <c r="B77" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="9"/>
-      <c r="B78" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="9" t="s">
+    <row r="98" spans="1:4">
+      <c r="A98" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="13"/>
+      <c r="B99" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="13"/>
+      <c r="B100" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="13"/>
+      <c r="B101" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="13"/>
+      <c r="B102" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="13"/>
+      <c r="B103" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="13"/>
+      <c r="B105" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="13"/>
+      <c r="B106" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="13"/>
+      <c r="B107" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="13"/>
+      <c r="B108" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="13"/>
+      <c r="B109" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="13"/>
+      <c r="B110" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="13"/>
+      <c r="B112" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A113" s="14"/>
+      <c r="B113" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="14.65" thickBot="1"/>
+    <row r="116" spans="1:4">
+      <c r="A116" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="B79" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D79" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="9"/>
-      <c r="B80" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="9"/>
-      <c r="B81" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D81" s="10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="9"/>
-      <c r="B82" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D82" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="9"/>
-      <c r="B83" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D83" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="9"/>
-      <c r="B84" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D84" s="10" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="9"/>
-      <c r="B85" s="14" t="s">
-        <v>353</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="B86" s="3" t="s">
+      <c r="B116" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C116" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="D86" s="10" t="s">
+      <c r="D116" s="21" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="9"/>
-      <c r="B87" s="3" t="s">
+    <row r="117" spans="1:4">
+      <c r="A117" s="13"/>
+      <c r="B117" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C117" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D87" s="10" t="s">
+      <c r="D117" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="9"/>
-      <c r="B88" s="3" t="s">
+    <row r="118" spans="1:4">
+      <c r="A118" s="13"/>
+      <c r="B118" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C118" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D88" s="10" t="s">
+      <c r="D118" s="5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="9"/>
-      <c r="B89" s="3" t="s">
+    <row r="119" spans="1:4">
+      <c r="A119" s="13"/>
+      <c r="B119" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C119" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D89" s="10" t="s">
+      <c r="D119" s="5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="9"/>
-      <c r="B90" s="3" t="s">
+    <row r="120" spans="1:4">
+      <c r="A120" s="13"/>
+      <c r="B120" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C120" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D90" s="10" t="s">
+      <c r="D120" s="5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D91" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="9"/>
-      <c r="B92" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D92" s="10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="9"/>
-      <c r="B93" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="D93" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="9"/>
-      <c r="B94" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D94" s="10" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="9"/>
-      <c r="B95" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="D95" s="10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="9"/>
-      <c r="B96" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="10" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="9" t="s">
-        <v>368</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D97" s="10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="9"/>
-      <c r="B98" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D98" s="10" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="9"/>
-      <c r="B99" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="D99" s="10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="9"/>
-      <c r="B100" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D100" s="10" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="9"/>
-      <c r="B101" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="9"/>
-      <c r="B102" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="D102" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D103" s="10" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="9"/>
-      <c r="B104" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="9"/>
-      <c r="B105" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D105" s="10" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="9"/>
-      <c r="B106" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D106" s="10" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="9"/>
-      <c r="B107" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D107" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="9"/>
-      <c r="B108" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D108" s="10" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="9" t="s">
+    <row r="121" spans="1:4">
+      <c r="A121" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="B109" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="D109" s="10" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="9"/>
-      <c r="B110" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="D110" s="10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="9"/>
-      <c r="B111" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="D111" s="10" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="9"/>
-      <c r="B112" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="D112" s="10" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="9"/>
-      <c r="B113" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="D113" s="10" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="9"/>
-      <c r="B114" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D114" s="10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="9"/>
-      <c r="B115" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="D115" s="10" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="9" t="s">
-        <v>371</v>
-      </c>
-      <c r="B116" s="3" t="s">
+      <c r="B121" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C121" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D116" s="10" t="s">
+      <c r="D121" s="5" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="9"/>
-      <c r="B117" s="3" t="s">
+    <row r="122" spans="1:4">
+      <c r="A122" s="13"/>
+      <c r="B122" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C122" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D117" s="10" t="s">
+      <c r="D122" s="5" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="9"/>
-      <c r="B118" s="3" t="s">
+    <row r="123" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A123" s="14"/>
+      <c r="B123" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C123" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="D118" s="10" t="s">
+      <c r="D123" s="7" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="D119" s="10" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="9"/>
-      <c r="B120" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="D120" s="10" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="14.65" thickBot="1">
-      <c r="A121" s="11"/>
-      <c r="B121" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="C121" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="D121" s="13" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A109:A115"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="A71:A78"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="A86:A90"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A103:A108"/>
+    <mergeCell ref="A61:A70"/>
+    <mergeCell ref="A121:A123"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:A14"/>
     <mergeCell ref="A15:A32"/>
     <mergeCell ref="A33:A49"/>
     <mergeCell ref="A50:A60"/>
-    <mergeCell ref="A61:A70"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A111:A113"/>
+    <mergeCell ref="A71:A78"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="A116:A120"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A92:A97"/>
+    <mergeCell ref="A98:A103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding DataTypes+StructType in pysparkv2
</commit_message>
<xml_diff>
--- a/Databricks_Notes.xlsx
+++ b/Databricks_Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Confidential\data-cloudops-natvie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D3D00C-BC7C-41A4-B25E-06218ECAB371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD849BC-7ED0-4A76-A906-0FC57FF363D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{6D06DD71-AA96-4A60-BF7F-1C9189E66ACB}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="373">
-  <si>
-    <t>Databricks Performance Optimization Techniques</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="372">
   <si>
     <t>Category</t>
   </si>
@@ -3267,7 +3264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3288,16 +3285,8 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3307,12 +3296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3464,7 +3447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3502,32 +3485,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3846,10 +3817,11 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3860,1502 +3832,1493 @@
     <col min="4" max="4" width="79.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="28.5">
+      <c r="A2" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.5">
-      <c r="A3" s="13" t="s">
+      <c r="C2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="15"/>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="15"/>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="15"/>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="15"/>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="15"/>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="15"/>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="15"/>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="15"/>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="15"/>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="15"/>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.5">
+      <c r="A13" s="15"/>
+      <c r="B13" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="13"/>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="13"/>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="13"/>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="13"/>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="13"/>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="13"/>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="13"/>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="13"/>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="13"/>
-      <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="13"/>
-      <c r="B13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.5">
-      <c r="A14" s="13"/>
-      <c r="B14" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="15"/>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="15"/>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="15"/>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="15"/>
+      <c r="B18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="15"/>
+      <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="15"/>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="15"/>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="15"/>
+      <c r="B22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="15"/>
+      <c r="B23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="15"/>
+      <c r="B24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="15"/>
+      <c r="B25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="15"/>
+      <c r="B26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="15"/>
+      <c r="B27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="15"/>
+      <c r="B28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="15"/>
+      <c r="B29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="15"/>
+      <c r="B30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="15"/>
+      <c r="B31" s="8" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="13" t="s">
+      <c r="C31" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="13"/>
-      <c r="B16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="13"/>
-      <c r="B17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="13"/>
-      <c r="B18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="13"/>
-      <c r="B19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="13"/>
-      <c r="B20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="13"/>
-      <c r="B21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="13"/>
-      <c r="B22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="13"/>
-      <c r="B23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="13"/>
-      <c r="B24" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="13"/>
-      <c r="B25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="13"/>
-      <c r="B26" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="13"/>
-      <c r="B27" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="13"/>
-      <c r="B28" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="13"/>
-      <c r="B29" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="13"/>
-      <c r="B30" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="13"/>
-      <c r="B31" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="B32" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="13"/>
-      <c r="B32" s="8" t="s">
-        <v>335</v>
-      </c>
       <c r="C32" s="2" t="s">
-        <v>336</v>
+        <v>88</v>
       </c>
       <c r="D32" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="15"/>
+      <c r="B33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="15"/>
+      <c r="B34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="15"/>
+      <c r="B35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="15"/>
+      <c r="B36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="15"/>
+      <c r="B37" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="15"/>
+      <c r="B38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="15"/>
+      <c r="B39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="15"/>
+      <c r="B40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="15"/>
+      <c r="B41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="15"/>
+      <c r="B42" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="15"/>
+      <c r="B43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="15"/>
+      <c r="B44" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="15"/>
+      <c r="B45" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="15"/>
+      <c r="B46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="15"/>
+      <c r="B47" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="15"/>
+      <c r="B48" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="13" t="s">
+      <c r="C48" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="13"/>
-      <c r="B34" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="13"/>
-      <c r="B35" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="13"/>
-      <c r="B36" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="13"/>
-      <c r="B37" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="13"/>
-      <c r="B38" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="13"/>
-      <c r="B39" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="13"/>
-      <c r="B40" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="13"/>
-      <c r="B41" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B49" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="15"/>
+      <c r="B50" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="15"/>
+      <c r="B51" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="15"/>
+      <c r="B52" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="15"/>
+      <c r="B53" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="15"/>
+      <c r="B54" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="15"/>
+      <c r="B55" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="15"/>
+      <c r="B56" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="15"/>
+      <c r="B57" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="15"/>
+      <c r="B58" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="15"/>
+      <c r="B59" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="15"/>
+      <c r="B61" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="13"/>
-      <c r="B42" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="13"/>
-      <c r="B43" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="13"/>
-      <c r="B44" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="13"/>
-      <c r="B45" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="13"/>
-      <c r="B46" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="13"/>
-      <c r="B47" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="13"/>
-      <c r="B48" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="13"/>
-      <c r="B49" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="13"/>
-      <c r="B51" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="13"/>
-      <c r="B52" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="13"/>
-      <c r="B53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="13"/>
-      <c r="B54" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="13"/>
-      <c r="B55" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="13"/>
-      <c r="B56" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="13"/>
-      <c r="B57" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="13"/>
-      <c r="B58" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="13"/>
-      <c r="B59" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="13"/>
-      <c r="B60" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D60" s="5" t="s">
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="15"/>
+      <c r="B62" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="15"/>
+      <c r="B63" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="15"/>
+      <c r="B64" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="15"/>
+      <c r="B65" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="15"/>
+      <c r="B66" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="15"/>
+      <c r="B67" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="15"/>
+      <c r="B68" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="15"/>
+      <c r="B69" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="13" t="s">
+      <c r="C69" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="13"/>
-      <c r="B62" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="13"/>
-      <c r="B63" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="13"/>
-      <c r="B64" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="13"/>
-      <c r="B65" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="13"/>
-      <c r="B66" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="13"/>
-      <c r="B67" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="13"/>
-      <c r="B68" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="13"/>
-      <c r="B69" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D69" s="5" t="s">
+      <c r="B70" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="13"/>
-      <c r="B70" s="18" t="s">
-        <v>344</v>
-      </c>
       <c r="C70" s="2" t="s">
-        <v>345</v>
+        <v>191</v>
       </c>
       <c r="D70" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="15"/>
+      <c r="B71" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="15"/>
+      <c r="B72" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="15"/>
+      <c r="B73" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="15"/>
+      <c r="B74" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D74" s="5" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="13"/>
-      <c r="B72" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="13"/>
-      <c r="B73" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="13"/>
-      <c r="B74" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="13"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="13"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D76" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="15"/>
+      <c r="B77" s="2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="13"/>
-      <c r="B77" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="C77" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="13"/>
-      <c r="B78" s="18" t="s">
-        <v>349</v>
-      </c>
       <c r="C78" s="2" t="s">
-        <v>350</v>
+        <v>209</v>
       </c>
       <c r="D78" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="15"/>
+      <c r="B79" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="15"/>
+      <c r="B80" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="15"/>
+      <c r="B81" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="15"/>
+      <c r="B82" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="15"/>
+      <c r="B83" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="15"/>
+      <c r="B84" s="2" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="13" t="s">
+      <c r="C84" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="15"/>
+      <c r="B86" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="15"/>
+      <c r="B87" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="15"/>
+      <c r="B88" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="15"/>
+      <c r="B89" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="15"/>
+      <c r="B90" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="15"/>
+      <c r="B92" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="15"/>
+      <c r="B93" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="15"/>
+      <c r="B94" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="15"/>
+      <c r="B95" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="15"/>
+      <c r="B96" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="15"/>
+      <c r="B98" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="15"/>
+      <c r="B99" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="15"/>
+      <c r="B100" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="15"/>
+      <c r="B101" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="15"/>
+      <c r="B102" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="15"/>
+      <c r="B104" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="15"/>
+      <c r="B105" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="15"/>
+      <c r="B106" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="15"/>
+      <c r="B107" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="15"/>
+      <c r="B108" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="15"/>
+      <c r="B109" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="15"/>
+      <c r="B111" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A112" s="16"/>
+      <c r="B112" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="14.65" thickBot="1"/>
+    <row r="115" spans="1:4">
+      <c r="A115" s="17" t="s">
         <v>364</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="13"/>
-      <c r="B80" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="13"/>
-      <c r="B81" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="13"/>
-      <c r="B82" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="13"/>
-      <c r="B83" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="13"/>
-      <c r="B84" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D84" s="5" t="s">
+      <c r="B115" s="13" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="13"/>
-      <c r="B85" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="13"/>
-      <c r="B87" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="13"/>
-      <c r="B88" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="13"/>
-      <c r="B89" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="13"/>
-      <c r="B90" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="13"/>
-      <c r="B91" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="13"/>
-      <c r="B93" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="13"/>
-      <c r="B94" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="13"/>
-      <c r="B95" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="13"/>
-      <c r="B96" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="13"/>
-      <c r="B97" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="13"/>
-      <c r="B99" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="13"/>
-      <c r="B100" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="13"/>
-      <c r="B101" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="13"/>
-      <c r="B102" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="13"/>
-      <c r="B103" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="13" t="s">
+      <c r="C115" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="15"/>
+      <c r="B116" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="15"/>
+      <c r="B117" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="15"/>
+      <c r="B118" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="15"/>
+      <c r="B119" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="13"/>
-      <c r="B105" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="13"/>
-      <c r="B106" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="13"/>
-      <c r="B107" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="13"/>
-      <c r="B108" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="13"/>
-      <c r="B109" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D109" s="5" t="s">
+      <c r="B120" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="13"/>
-      <c r="B110" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="13"/>
-      <c r="B112" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="D112" s="5" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="14.65" thickBot="1">
-      <c r="A113" s="14"/>
-      <c r="B113" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="D113" s="7" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="14.65" thickBot="1"/>
-    <row r="116" spans="1:4">
-      <c r="A116" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="B116" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="C116" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="D116" s="21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="13"/>
-      <c r="B117" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="13"/>
-      <c r="B118" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="13"/>
-      <c r="B119" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D119" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="13"/>
-      <c r="B120" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="C120" s="2" t="s">
-        <v>240</v>
+        <v>313</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>241</v>
+        <v>314</v>
       </c>
     </row>
     <row r="121" spans="1:4">
-      <c r="A121" s="13" t="s">
-        <v>370</v>
-      </c>
+      <c r="A121" s="15"/>
       <c r="B121" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="13"/>
-      <c r="B122" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C122" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D122" s="5" t="s">
+    </row>
+    <row r="122" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A122" s="16"/>
+      <c r="B122" s="6" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="14.65" thickBot="1">
-      <c r="A123" s="14"/>
-      <c r="B123" s="6" t="s">
+      <c r="C122" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="C123" s="6" t="s">
+      <c r="D122" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="D123" s="7" t="s">
-        <v>321</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A61:A70"/>
-    <mergeCell ref="A121:A123"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A14"/>
-    <mergeCell ref="A15:A32"/>
-    <mergeCell ref="A33:A49"/>
-    <mergeCell ref="A50:A60"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A111:A113"/>
-    <mergeCell ref="A71:A78"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="A116:A120"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A92:A97"/>
-    <mergeCell ref="A98:A103"/>
+  <mergeCells count="14">
+    <mergeCell ref="A60:A69"/>
+    <mergeCell ref="A120:A122"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A31"/>
+    <mergeCell ref="A32:A48"/>
+    <mergeCell ref="A49:A59"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="A70:A77"/>
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="A115:A119"/>
+    <mergeCell ref="A85:A90"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A97:A102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>